<commit_message>
Added jupyter lab notebooks in Pandas
</commit_message>
<xml_diff>
--- a/training_schedule.xlsx
+++ b/training_schedule.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jony0\Downloads\CV_training\CV_training\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46D236BF-9EB8-4E60-9FF6-4D08D1935AC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E172E3FD-73F7-4055-A206-DCA7DD36ED52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -453,8 +453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -512,7 +512,7 @@
       </c>
       <c r="D5">
         <f>SUM(D6:D11)</f>
-        <v>1</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
@@ -543,6 +543,9 @@
       </c>
       <c r="C8">
         <v>6.5</v>
+      </c>
+      <c r="D8">
+        <v>5.5</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Commit of DS Part 1
</commit_message>
<xml_diff>
--- a/training_schedule.xlsx
+++ b/training_schedule.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jony0\Downloads\CV_training\CV_training\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E172E3FD-73F7-4055-A206-DCA7DD36ED52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDA61D01-587E-4920-98B1-7EDE1592E898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -453,8 +453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -512,7 +512,7 @@
       </c>
       <c r="D5">
         <f>SUM(D6:D11)</f>
-        <v>6.5</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
@@ -555,6 +555,9 @@
       <c r="C9">
         <v>1</v>
       </c>
+      <c r="D9">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
@@ -563,6 +566,9 @@
       <c r="C10">
         <v>2</v>
       </c>
+      <c r="D10">
+        <v>2.5</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
@@ -582,7 +588,7 @@
       </c>
       <c r="D12">
         <f>SUM(D13:D20)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
@@ -592,6 +598,9 @@
       <c r="C13">
         <v>1</v>
       </c>
+      <c r="D13">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
@@ -599,6 +608,9 @@
       </c>
       <c r="C14">
         <v>1</v>
+      </c>
+      <c r="D14">
+        <v>0.5</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>